<commit_message>
BC ammi results added
</commit_message>
<xml_diff>
--- a/output/2022_pacific_master_results_BC_2024-01-23_.xlsx
+++ b/output/2022_pacific_master_results_BC_2024-01-23_.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cgiar-my.sharepoint.com/personal/luis_delgado_cgiar_org/Documents/Data Analysis/agrosavia_pacific/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_C8BCC003F9E28E974791967ABD2AA3872E856F29" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F8A5B1C-2B3D-471B-8188-A7152D98DC63}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="11_C8BCC003F9E28E974791967ABD2AA3872E856F29" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{083A40EE-A05D-43CC-BED3-1935724624D7}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="8" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="8" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mean_of_sd" sheetId="1" r:id="rId1"/>
@@ -371,7 +371,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -379,12 +379,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1070,9 +1086,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="180" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.7265625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -9858,8 +9879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView zoomScale="115" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9868,118 +9889,120 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>5</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>380.63400000000001</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>76.126999999999995</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>1.0640000000000001</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="1">
         <v>0.39200000000000002</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>3</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>1728.384</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>576.12800000000004</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>8.0500000000000007</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>1</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>858.75099999999998</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>858.75099999999998</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>11.999000000000001</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="1">
         <v>1E-3</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>10</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>419.31299999999999</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>41.930999999999997</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>0.58599999999999997</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="1">
         <v>0.81699999999999995</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>47</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>3363.7570000000001</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>71.569000000000003</v>
       </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>